<commit_message>
Navigate between rows tests
</commit_message>
<xml_diff>
--- a/tests/Spreadsheet/test.xlsx
+++ b/tests/Spreadsheet/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -256,8 +256,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Color tests(Bad, very bad)
</commit_message>
<xml_diff>
--- a/tests/Spreadsheet/test.xlsx
+++ b/tests/Spreadsheet/test.xlsx
@@ -80,7 +80,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +111,12 @@
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -118,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -140,6 +146,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="5" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="6" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1495,10 +1505,10 @@
       </c>
     </row>
     <row r="2" spans="1:1025" customHeight="1" ht="12.8">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1">
@@ -1512,10 +1522,10 @@
       </c>
     </row>
     <row r="3" spans="1:1025" customHeight="1" ht="12.8">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1">

</xml_diff>